<commit_message>
Starting leafout to parallel nonleafout analysis
</commit_message>
<xml_diff>
--- a/analyses/Summary of Nonleafout.xlsx
+++ b/analyses/Summary of Nonleafout.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>ACEPEN</t>
   </si>
@@ -163,6 +163,18 @@
   </si>
   <si>
     <t>Slightly more nl in HF</t>
+  </si>
+  <si>
+    <t>- more nl in SH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">more nl at chill1 </t>
+  </si>
+  <si>
+    <t>more nl at chill2</t>
+  </si>
+  <si>
+    <t>marginal: warmxchillxsite. At HF, most nl at chill1 in cool.</t>
   </si>
 </sst>
 </file>
@@ -227,7 +239,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -237,6 +249,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -575,7 +588,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -667,9 +680,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="45">
+    <row r="5" spans="1:13" ht="60">
       <c r="A5" t="s">
         <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>37</v>
@@ -735,6 +754,12 @@
     <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>9</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" t="s">
+        <v>50</v>
       </c>
       <c r="H12" s="2"/>
       <c r="K12" s="2"/>

</xml_diff>

<commit_message>
Updates to text, starting Stan model work again
</commit_message>
<xml_diff>
--- a/analyses/Summary of Nonleafout.xlsx
+++ b/analyses/Summary of Nonleafout.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
@@ -588,7 +588,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>